<commit_message>
Backup QR Scanner data - 2025-12-21T17:43:34.584Z - Cache Bust: 1766339014584
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Psychiatry_scanner1766053804167_272efcfda7bd3208e090f05a24198cc42a8b7c15230d58e6534a6eec0a74da5a.xlsx
+++ b/log_history/Y4_B2526_Psychiatry_scanner1766053804167_272efcfda7bd3208e090f05a24198cc42a8b7c15230d58e6534a6eec0a74da5a.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Psychiatry" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1202,29 +1202,9 @@
         <v>160715@med.asu.edu.eg</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="str">
-        <v>190975</v>
-      </c>
-      <c r="B41" t="str">
-        <v>Psychiatry</v>
-      </c>
-      <c r="C41" t="str">
-        <v>18/12/2025</v>
-      </c>
-      <c r="D41" t="str">
-        <v>12:37:41</v>
-      </c>
-      <c r="E41" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F41" t="str">
-        <v>160715@med.asu.edu.eg</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F41"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F40"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>